<commit_message>
New graphics added and better organization
Finally figures added to the project.
</commit_message>
<xml_diff>
--- a/info_used.xlsx
+++ b/info_used.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive\Desktop\DeleteMe\Streamlit_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fruguitos\Desktop\DeleteMe\Streamlit_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A89D2C-9D73-4BC9-B80C-7D9746E445A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5233A1F-D392-4A30-B310-833AAD396BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FB7A556-ECDB-4209-B4E1-66CB754770F6}"/>
   </bookViews>
@@ -365,7 +365,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +426,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -455,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,6 +548,36 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -544,7 +598,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -842,11 +896,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A36E295-4D7D-47E0-801D-C873552FA26F}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.44140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="84.6640625" style="3" customWidth="1"/>
@@ -932,74 +986,74 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="27">
         <v>12</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="6" t="s">
+      <c r="C6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="31">
+        <v>4</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9">
-        <v>4</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="6" t="s">
+      <c r="C7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="31">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9">
-        <v>4</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="6" t="s">
+      <c r="C8" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="31">
+        <v>4</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="29" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1292,254 +1346,254 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="9">
-        <v>4</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="6" t="s">
+      <c r="C25" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="27">
+        <v>4</v>
+      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="9">
-        <v>4</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="6" t="s">
+      <c r="C26" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="27">
+        <v>4</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="9">
-        <v>4</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="6" t="s">
+      <c r="C27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="27">
+        <v>4</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="9">
-        <v>4</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="6" t="s">
+      <c r="C28" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="27">
+        <v>4</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="9">
-        <v>4</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="6" t="s">
+      <c r="C29" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="31">
+        <v>4</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="9">
-        <v>4</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="6" t="s">
+      <c r="C30" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="31">
+        <v>4</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="9">
-        <v>4</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="6" t="s">
+      <c r="C31" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="31">
+        <v>4</v>
+      </c>
+      <c r="E31" s="32"/>
+      <c r="F31" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="9">
-        <v>4</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="6" t="s">
+      <c r="C32" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="31">
+        <v>4</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="9">
-        <v>4</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="6" t="s">
+      <c r="C33" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="31">
+        <v>4</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="9">
-        <v>4</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="6" t="s">
+      <c r="C34" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="31">
+        <v>4</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="9">
-        <v>4</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="6" t="s">
+      <c r="C35" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="31">
+        <v>4</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="9">
-        <v>4</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="6" t="s">
+      <c r="C36" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="31">
+        <v>4</v>
+      </c>
+      <c r="E36" s="32"/>
+      <c r="F36" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="9">
-        <v>4</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="6" t="s">
+      <c r="C37" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="31">
+        <v>4</v>
+      </c>
+      <c r="E37" s="32"/>
+      <c r="F37" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="9">
-        <v>4</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="6" t="s">
+      <c r="C38" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="31">
+        <v>4</v>
+      </c>
+      <c r="E38" s="32"/>
+      <c r="F38" s="29" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1563,6 +1617,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>